<commit_message>
Update 1.5.7.1: Bug fixes and QoL
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта СТВТ.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта СТВТ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F27F1B-DB51-4481-A0C2-831558F88615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C08E180-EFC6-46F6-AF17-036A0C9A4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="СТВТ" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,7 +484,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B159" xr:uid="{97E180B8-70D3-40D7-9813-50FDDD79F612}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B159 B2" xr:uid="{97E180B8-70D3-40D7-9813-50FDDD79F612}">
       <formula1>"  В ожидании, Идет работа, Работа завершена,   Сдано заказчику,"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{4B475DF3-5C0A-4DF1-A459-425E73B3B6A8}">
@@ -517,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5071E1-C0DA-4876-87DF-F8108C1EBEAA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
+    <sheetView zoomScale="193" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>